<commit_message>
Add script for analyzing missingness in the data
</commit_message>
<xml_diff>
--- a/data/Find Missingness.xlsx
+++ b/data/Find Missingness.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Documents\caps_anxiety\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6609D1A-A42D-462B-AADC-5D62E8D45BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C2290E-3324-44CB-A661-63FC68E87FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="130">
   <si>
     <t>demo_tb</t>
   </si>
@@ -393,13 +394,46 @@
   </si>
   <si>
     <t>csvs_demo</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t># Morning</t>
+  </si>
+  <si>
+    <t># Evening</t>
+  </si>
+  <si>
+    <t>First Day of Survey</t>
+  </si>
+  <si>
+    <t>Last Day of Survey</t>
+  </si>
+  <si>
+    <t># of Days</t>
+  </si>
+  <si>
+    <t>% Morning</t>
+  </si>
+  <si>
+    <t>% Evening</t>
+  </si>
+  <si>
+    <t>TOTAL on Evening_Survey =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% ID based on Evening_Survey = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL ID = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,8 +470,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,11 +502,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCFCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEAEAEA"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -469,27 +536,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y110"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +851,7 @@
     <col min="4" max="4" width="2.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.5546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="2.5546875" customWidth="1"/>
     <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.109375" customWidth="1"/>
@@ -795,36 +862,35 @@
     <col min="16" max="16" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
         <v>96</v>
       </c>
     </row>
@@ -847,19 +913,19 @@
       <c r="H2" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>105</v>
       </c>
       <c r="K2" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>98</v>
       </c>
       <c r="N2" t="s">
         <v>103</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -876,13 +942,13 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>61</v>
       </c>
       <c r="H3" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>98</v>
       </c>
       <c r="K3" t="s">
@@ -923,7 +989,7 @@
       <c r="K4" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="9" t="s">
         <v>61</v>
       </c>
       <c r="N4" t="s">
@@ -946,7 +1012,7 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
@@ -993,13 +1059,13 @@
       <c r="K6" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="N6" t="s">
         <v>103</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="6" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1051,7 +1117,7 @@
       <c r="E8" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="8" t="s">
         <v>55</v>
       </c>
       <c r="H8" t="s">
@@ -1086,7 +1152,7 @@
       <c r="E9" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>91</v>
       </c>
       <c r="H9" t="s">
@@ -1098,7 +1164,7 @@
       <c r="K9" t="s">
         <v>97</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="9" t="s">
         <v>55</v>
       </c>
       <c r="N9" t="s">
@@ -1133,7 +1199,7 @@
       <c r="K10" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="9" t="s">
         <v>91</v>
       </c>
       <c r="N10" t="s">
@@ -1194,7 +1260,7 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="1"/>
       <c r="H12" t="s">
         <v>113</v>
       </c>
@@ -1335,7 +1401,7 @@
       <c r="F16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="1"/>
       <c r="H16" t="s">
         <v>113</v>
       </c>
@@ -1371,7 +1437,7 @@
       <c r="F17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="1"/>
       <c r="H17" t="s">
         <v>113</v>
       </c>
@@ -1410,7 +1476,7 @@
       <c r="H18" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="5" t="s">
         <v>99</v>
       </c>
       <c r="K18" t="s">
@@ -1486,7 +1552,7 @@
       <c r="K20" t="s">
         <v>97</v>
       </c>
-      <c r="L20" s="9" t="s">
+      <c r="L20" s="6" t="s">
         <v>99</v>
       </c>
       <c r="N20" t="s">
@@ -1772,7 +1838,7 @@
       <c r="N28" t="s">
         <v>103</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="O28" s="6" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2039,7 +2105,7 @@
       <c r="H37" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="5" t="s">
         <v>100</v>
       </c>
       <c r="K37" t="s">
@@ -2097,7 +2163,7 @@
       <c r="K39" t="s">
         <v>97</v>
       </c>
-      <c r="L39" s="9" t="s">
+      <c r="L39" s="6" t="s">
         <v>100</v>
       </c>
       <c r="N39" t="s">
@@ -2273,7 +2339,7 @@
       <c r="H46" t="s">
         <v>113</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="5" t="s">
         <v>101</v>
       </c>
       <c r="K46" t="s">
@@ -2311,7 +2377,7 @@
       <c r="N47" t="s">
         <v>103</v>
       </c>
-      <c r="O47" s="9" t="s">
+      <c r="O47" s="6" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2331,7 +2397,7 @@
       <c r="K48" t="s">
         <v>97</v>
       </c>
-      <c r="L48" s="9" t="s">
+      <c r="L48" s="6" t="s">
         <v>101</v>
       </c>
       <c r="N48" t="s">
@@ -2545,7 +2611,7 @@
       <c r="N56" t="s">
         <v>103</v>
       </c>
-      <c r="O56" s="9" t="s">
+      <c r="O56" s="6" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3151,7 +3217,7 @@
       <c r="E80" t="s">
         <v>0</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="8" t="s">
         <v>67</v>
       </c>
       <c r="H80" t="s">
@@ -3209,7 +3275,7 @@
       <c r="H82" t="s">
         <v>113</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="I82" t="s">
         <v>19</v>
       </c>
       <c r="K82" t="s">
@@ -3235,7 +3301,7 @@
       <c r="H83" t="s">
         <v>113</v>
       </c>
-      <c r="I83" s="5" t="s">
+      <c r="I83" t="s">
         <v>71</v>
       </c>
       <c r="K83" t="s">
@@ -3267,7 +3333,7 @@
       <c r="K84" t="s">
         <v>97</v>
       </c>
-      <c r="L84" s="13" t="s">
+      <c r="L84" s="9" t="s">
         <v>67</v>
       </c>
       <c r="N84" t="s">
@@ -3359,7 +3425,7 @@
       <c r="E88" t="s">
         <v>0</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H88" t="s">
@@ -3475,7 +3541,7 @@
       <c r="K92" t="s">
         <v>97</v>
       </c>
-      <c r="L92" s="13" t="s">
+      <c r="L92" s="9" t="s">
         <v>6</v>
       </c>
       <c r="N92" t="s">
@@ -3495,7 +3561,7 @@
       <c r="H93" t="s">
         <v>113</v>
       </c>
-      <c r="I93" s="8" t="s">
+      <c r="I93" s="5" t="s">
         <v>102</v>
       </c>
       <c r="K93" t="s">
@@ -3588,11 +3654,11 @@
         <f>COUNTA(F2:F95)</f>
         <v>94</v>
       </c>
-      <c r="G97" s="7"/>
+      <c r="G97" s="3"/>
       <c r="K97" t="s">
         <v>97</v>
       </c>
-      <c r="L97" s="9" t="s">
+      <c r="L97" s="6" t="s">
         <v>102</v>
       </c>
       <c r="N97" t="s">
@@ -3694,7 +3760,7 @@
       <c r="N105" t="s">
         <v>103</v>
       </c>
-      <c r="O105" s="9" t="s">
+      <c r="O105" s="6" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3734,4 +3800,1125 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3002DECB-CE0C-487A-8D7E-F19DE7DD833E}">
+  <dimension ref="A1:H100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>172</v>
+      </c>
+      <c r="C2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+      <c r="C3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>226</v>
+      </c>
+      <c r="C4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>151</v>
+      </c>
+      <c r="C6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>176</v>
+      </c>
+      <c r="C7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>219</v>
+      </c>
+      <c r="C10">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>92</v>
+      </c>
+      <c r="C11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>165</v>
+      </c>
+      <c r="C13">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>241</v>
+      </c>
+      <c r="C15">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>113</v>
+      </c>
+      <c r="C16">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>197</v>
+      </c>
+      <c r="C17">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>235</v>
+      </c>
+      <c r="C18">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>175</v>
+      </c>
+      <c r="C19">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>59</v>
+      </c>
+      <c r="C20">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>110</v>
+      </c>
+      <c r="C22">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>75</v>
+      </c>
+      <c r="C24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>107</v>
+      </c>
+      <c r="C25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>197</v>
+      </c>
+      <c r="C26">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>61</v>
+      </c>
+      <c r="C27">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>86</v>
+      </c>
+      <c r="C28">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>134</v>
+      </c>
+      <c r="C29">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>193</v>
+      </c>
+      <c r="C30">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>162</v>
+      </c>
+      <c r="C32">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>250</v>
+      </c>
+      <c r="C34">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>252</v>
+      </c>
+      <c r="C35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>143</v>
+      </c>
+      <c r="C36">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>242</v>
+      </c>
+      <c r="C37">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>191</v>
+      </c>
+      <c r="C39">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>143</v>
+      </c>
+      <c r="C40">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>183</v>
+      </c>
+      <c r="C41">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>161</v>
+      </c>
+      <c r="C42">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>248</v>
+      </c>
+      <c r="C43">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>96</v>
+      </c>
+      <c r="C44">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>173</v>
+      </c>
+      <c r="C45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>257</v>
+      </c>
+      <c r="C46">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>172</v>
+      </c>
+      <c r="C48">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>213</v>
+      </c>
+      <c r="C49">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>116</v>
+      </c>
+      <c r="C50">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>42</v>
+      </c>
+      <c r="C52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>168</v>
+      </c>
+      <c r="C53">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>214</v>
+      </c>
+      <c r="C54">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>247</v>
+      </c>
+      <c r="C55">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>45</v>
+      </c>
+      <c r="C56">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>237</v>
+      </c>
+      <c r="C57">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>244</v>
+      </c>
+      <c r="C58">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>161</v>
+      </c>
+      <c r="C59">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>259</v>
+      </c>
+      <c r="C60">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>221</v>
+      </c>
+      <c r="C61">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>113</v>
+      </c>
+      <c r="C63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>126</v>
+      </c>
+      <c r="C64">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>53</v>
+      </c>
+      <c r="C65">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>253</v>
+      </c>
+      <c r="C66">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>213</v>
+      </c>
+      <c r="C67">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>113</v>
+      </c>
+      <c r="C68">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>117</v>
+      </c>
+      <c r="C69">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>75</v>
+      </c>
+      <c r="C70">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>234</v>
+      </c>
+      <c r="C71">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>107</v>
+      </c>
+      <c r="C72">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>162</v>
+      </c>
+      <c r="C73">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>93</v>
+      </c>
+      <c r="C74">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>223</v>
+      </c>
+      <c r="C75">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>81</v>
+      </c>
+      <c r="C76">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>166</v>
+      </c>
+      <c r="C77">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>146</v>
+      </c>
+      <c r="C78">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>161</v>
+      </c>
+      <c r="C80">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>229</v>
+      </c>
+      <c r="C81">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>110</v>
+      </c>
+      <c r="C82">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>59</v>
+      </c>
+      <c r="C83">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>199</v>
+      </c>
+      <c r="C84">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>151</v>
+      </c>
+      <c r="C85">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>176</v>
+      </c>
+      <c r="C86">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>71</v>
+      </c>
+      <c r="C87">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>96</v>
+      </c>
+      <c r="C88">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>212</v>
+      </c>
+      <c r="C89">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>168</v>
+      </c>
+      <c r="C90">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>38</v>
+      </c>
+      <c r="C91">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>16</v>
+      </c>
+      <c r="C92">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>157</v>
+      </c>
+      <c r="C93">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>250</v>
+      </c>
+      <c r="C94">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>291</v>
+      </c>
+      <c r="C95">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>129</v>
+      </c>
+      <c r="B97">
+        <f>SUM(B2:B95)</f>
+        <v>13589</v>
+      </c>
+      <c r="C97">
+        <f>SUM(C2:C95)</f>
+        <v>13081</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>127</v>
+      </c>
+      <c r="B98">
+        <v>14491</v>
+      </c>
+      <c r="C98">
+        <v>13746</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100">
+        <f>B97/B98</f>
+        <v>0.93775446829066322</v>
+      </c>
+      <c r="C100">
+        <f>C97/C98</f>
+        <v>0.95162229012076238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>